<commit_message>
Added UI for hero and enemies
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Hallam\Desktop\TAGD\CallOfDionysus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90FB13D-2F1F-456D-8520-03DC60B0522B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FEB3BA-674F-4A57-B7C9-2F455D58B65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
   <si>
     <t>Task</t>
   </si>
@@ -742,17 +742,17 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="43.41015625" customWidth="1"/>
-    <col min="3" max="3" width="21.703125" customWidth="1"/>
-    <col min="4" max="4" width="24.05859375" customWidth="1"/>
-    <col min="5" max="5" width="9.52734375" customWidth="1"/>
-    <col min="6" max="6" width="29.46875" customWidth="1"/>
-    <col min="7" max="7" width="29.17578125" customWidth="1"/>
+    <col min="1" max="1" width="43.41796875" customWidth="1"/>
+    <col min="3" max="3" width="21.68359375" customWidth="1"/>
+    <col min="4" max="4" width="24.05078125" customWidth="1"/>
+    <col min="5" max="5" width="9.5234375" customWidth="1"/>
+    <col min="6" max="6" width="29.47265625" customWidth="1"/>
+    <col min="7" max="7" width="29.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -772,7 +772,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -796,7 +796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -820,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>44</v>
       </c>
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -868,7 +868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="13" t="s">
         <v>39</v>
       </c>
@@ -892,7 +892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -916,7 +916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
@@ -940,7 +940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -953,7 +953,9 @@
       <c r="D9" s="3">
         <v>44608</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" t="s">
         <v>52</v>
@@ -962,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
@@ -975,7 +977,9 @@
       <c r="D10" s="3">
         <v>44608</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" t="s">
         <v>53</v>
@@ -984,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -1006,7 +1010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="14" t="s">
         <v>31</v>
       </c>
@@ -1022,7 +1026,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
@@ -1040,7 +1044,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -1058,7 +1062,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11" t="s">
         <v>22</v>
       </c>
@@ -1074,7 +1078,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
@@ -1090,7 +1094,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
@@ -1108,7 +1112,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="11" t="s">
         <v>55</v>
       </c>
@@ -1126,7 +1130,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -1139,10 +1143,12 @@
       <c r="D19" s="3">
         <v>44608</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="14" t="s">
         <v>60</v>
       </c>
@@ -1160,7 +1166,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="14" t="s">
         <v>61</v>
       </c>
@@ -1176,11 +1182,11 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -1196,7 +1202,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="14" t="s">
         <v>34</v>
       </c>
@@ -1212,7 +1218,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="11" t="s">
         <v>48</v>
       </c>
@@ -1228,7 +1234,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="11" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1250,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="12" t="s">
         <v>11</v>
       </c>
@@ -1260,7 +1266,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="13" t="s">
         <v>40</v>
       </c>
@@ -1276,7 +1282,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="13" t="s">
         <v>43</v>
       </c>
@@ -1292,7 +1298,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
@@ -1308,7 +1314,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="11" t="s">
         <v>19</v>
       </c>
@@ -1324,7 +1330,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="11" t="s">
         <v>25</v>
       </c>
@@ -1340,7 +1346,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="14" t="s">
         <v>33</v>
       </c>
@@ -1356,7 +1362,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="11" t="s">
         <v>26</v>
       </c>
@@ -1372,7 +1378,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="11" t="s">
         <v>37</v>
       </c>
@@ -1388,7 +1394,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="12" t="s">
         <v>45</v>
       </c>
@@ -1404,7 +1410,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="14" t="s">
         <v>32</v>
       </c>
@@ -1420,7 +1426,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -1428,7 +1434,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="12" t="s">
         <v>12</v>
       </c>
@@ -1444,7 +1450,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="11" t="s">
         <v>23</v>
       </c>
@@ -1460,7 +1466,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="11" t="s">
         <v>24</v>
       </c>
@@ -1476,7 +1482,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="12" t="s">
         <v>27</v>
       </c>
@@ -1492,7 +1498,7 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="14" t="s">
         <v>28</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>44650</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="13" t="s">
         <v>41</v>
       </c>
@@ -1520,7 +1526,7 @@
         <v>44650</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="13" t="s">
         <v>42</v>
       </c>
@@ -1534,7 +1540,7 @@
         <v>44650</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="12" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Added more sanity effects
Added sanity camera effects
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Hallam\Desktop\TAGD\CallOfDionysus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E86252-7B34-4D6F-A2A0-4E6B91EDD7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51409CFE-685C-425A-90CC-2F153453DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,7 +742,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1213,7 +1213,7 @@
         <v>44615</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F23" s="1"/>
     </row>

</xml_diff>

<commit_message>
Fixed knockback, added sanity consequences
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Hallam\Desktop\TAGD\CallOfDionysus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51409CFE-685C-425A-90CC-2F153453DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C846C8A5-68BE-48EA-81FE-19A1864969E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1213,7 +1213,7 @@
         <v>44615</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -1363,7 +1363,7 @@
         <v>44622</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added ghost animations, started sanity feedback
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Hallam\Desktop\TAGD\CallOfDionysus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C846C8A5-68BE-48EA-81FE-19A1864969E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AA80BF-6FA4-43BD-916B-7AF80AEFE36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>Task</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>2/23/2022- DELAYED</t>
+  </si>
+  <si>
+    <t>Player attacked animation</t>
+  </si>
+  <si>
+    <t>Ghost attacked animation</t>
   </si>
 </sst>
 </file>
@@ -741,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1032,6 +1038,12 @@
         <v>57</v>
       </c>
       <c r="F12" s="1"/>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11" t="s">
@@ -1050,6 +1062,12 @@
         <v>57</v>
       </c>
       <c r="F13" s="1"/>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="11" t="s">
@@ -1296,7 +1314,9 @@
       <c r="D28" s="5">
         <v>44615</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1312,7 +1332,9 @@
       <c r="D29" s="5">
         <v>44615</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1363,7 +1385,7 @@
         <v>44622</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added sanity message scripts
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Hallam\Desktop\TAGD\CallOfDionysus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AA80BF-6FA4-43BD-916B-7AF80AEFE36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12558DDE-2596-4C5B-B25E-F04577FCDAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
   <si>
     <t>Task</t>
   </si>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1266,7 +1266,9 @@
       <c r="D25" s="5">
         <v>44615</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1315,7 +1317,7 @@
         <v>44615</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -1333,7 +1335,7 @@
         <v>44615</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -1385,7 +1387,7 @@
         <v>44622</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Started updating based on playtesting feedback
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Hallam\Desktop\TAGD\CallOfDionysus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9FBF60-BD7C-4B29-8375-41075DE06172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9062022-CB2D-4094-9FF7-4FD79B27386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="79">
   <si>
     <t>Task</t>
   </si>
@@ -229,6 +229,39 @@
   </si>
   <si>
     <t>CUT</t>
+  </si>
+  <si>
+    <t>PLAYTESTING FEEDBACK GOALS</t>
+  </si>
+  <si>
+    <t>Add knock back to hero</t>
+  </si>
+  <si>
+    <t>Add pathfinding to ghosts</t>
+  </si>
+  <si>
+    <t>Make camera speed proportional to hero speed</t>
+  </si>
+  <si>
+    <t>Make sanity/hp reset per level</t>
+  </si>
+  <si>
+    <t>Make sanity wobble more punishing</t>
+  </si>
+  <si>
+    <t>Make UI more obvious</t>
+  </si>
+  <si>
+    <t>Invest in shaders</t>
+  </si>
+  <si>
+    <t>Noise indicator for taking damage</t>
+  </si>
+  <si>
+    <t>Pause spawners while at altars</t>
+  </si>
+  <si>
+    <t>Fix font in sanity messages</t>
   </si>
 </sst>
 </file>
@@ -762,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -932,7 +965,7 @@
         <v>44608</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" t="s">
@@ -1139,8 +1172,11 @@
         <v>57</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="14" t="s">
         <v>58</v>
       </c>
@@ -1157,8 +1193,17 @@
         <v>57</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18" s="14" t="s">
         <v>59</v>
       </c>
@@ -1175,12 +1220,27 @@
         <v>57</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" s="14" t="s">
         <v>33</v>
       </c>
@@ -1197,8 +1257,17 @@
         <v>57</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="14" t="s">
         <v>28</v>
       </c>
@@ -1215,8 +1284,17 @@
         <v>57</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" s="14" t="s">
         <v>29</v>
       </c>
@@ -1233,8 +1311,14 @@
         <v>57</v>
       </c>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -1251,8 +1335,14 @@
         <v>57</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" s="14" t="s">
         <v>32</v>
       </c>
@@ -1269,8 +1359,14 @@
         <v>57</v>
       </c>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25" s="11" t="s">
         <v>46</v>
       </c>
@@ -1287,8 +1383,17 @@
         <v>57</v>
       </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26" s="11" t="s">
         <v>5</v>
       </c>
@@ -1305,8 +1410,17 @@
         <v>57</v>
       </c>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A27" s="12" t="s">
         <v>11</v>
       </c>
@@ -1319,10 +1433,12 @@
       <c r="D27" s="5">
         <v>44615</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" s="19" t="s">
         <v>38</v>
       </c>
@@ -1340,7 +1456,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29" s="19" t="s">
         <v>41</v>
       </c>
@@ -1358,7 +1474,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30" s="11" t="s">
         <v>62</v>
       </c>
@@ -1376,7 +1492,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31" s="11" t="s">
         <v>63</v>
       </c>
@@ -1394,7 +1510,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A32" s="11" t="s">
         <v>23</v>
       </c>
@@ -1519,7 +1635,9 @@
       <c r="D39" s="10">
         <v>44650</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Added sounds and animation
</commit_message>
<xml_diff>
--- a/Sprint Plan.xlsx
+++ b/Sprint Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Hallam\Desktop\TAGD\CallOfDionysus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9062022-CB2D-4094-9FF7-4FD79B27386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ACB604-A658-4599-81E8-192BE5263383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
   <si>
     <t>Task</t>
   </si>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1226,6 +1226,9 @@
       <c r="H18">
         <v>1</v>
       </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="E19" s="1"/>
@@ -1317,6 +1320,9 @@
       <c r="H22">
         <v>1</v>
       </c>
+      <c r="I22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="11" t="s">
@@ -1365,6 +1371,9 @@
       <c r="H24">
         <v>1</v>
       </c>
+      <c r="I24" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25" s="11" t="s">
@@ -1488,7 +1497,7 @@
         <v>44622</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -1593,7 +1602,9 @@
       <c r="D36" s="7">
         <v>44629</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.5">
@@ -1653,7 +1664,9 @@
       <c r="D40" s="10">
         <v>44650</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.5">

</xml_diff>